<commit_message>
Ajout du layout (header, contentpage) et remplissage du journal de travail
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_GolazNicola.xlsx
+++ b/Journal-de-Travail_GolazNicola.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po42oio\Documents\GitHub\P_appMaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3872B11E-8163-4758-9B93-2E6FBABCFE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA2DD64-ECEA-4311-AD2A-679D58986442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="3315" windowWidth="24630" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1335" yWindow="915" windowWidth="24630" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t>Ajout de la tabbar a l'application, lecture de la docs de maui</t>
+  </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Recherche de comment organiser mes pages (layout)</t>
+  </si>
+  <si>
+    <t>Mise en place du layout (header, content et footer)</t>
+  </si>
+  <si>
+    <t>Début de l'affichage des livres, et recherche sur comment implémenter le backend</t>
   </si>
 </sst>
 </file>
@@ -1073,13 +1085,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.25E-2</c:v>
+                  <c:v>0.13541666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.375E-2</c:v>
+                  <c:v>0.11458333333333333</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2008,7 +2020,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2061,7 +2073,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 45 minutes</v>
+        <v>0 jours 9 heurs 0 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2076,15 +2088,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>360</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>405</v>
+        <v>540</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2263,15 +2275,19 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="46"/>
+        <v>15</v>
+      </c>
+      <c r="B12" s="46">
+        <v>45754</v>
+      </c>
       <c r="C12" s="47"/>
       <c r="D12" s="48"/>
       <c r="E12" s="49"/>
-      <c r="F12" s="36"/>
+      <c r="F12" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="55"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -2284,15 +2300,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="str">
+      <c r="A13" s="16">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B13" s="50">
+        <v>45775</v>
+      </c>
       <c r="C13" s="51"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="52">
+        <v>30</v>
+      </c>
+      <c r="E13" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>35</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="M13" t="s">
         <v>8</v>
@@ -2305,15 +2329,23 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="str">
+      <c r="A14" s="8">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="46"/>
-      <c r="C14" s="47"/>
+        <v>18</v>
+      </c>
+      <c r="B14" s="46">
+        <v>45775</v>
+      </c>
+      <c r="C14" s="47">
+        <v>1</v>
+      </c>
       <c r="D14" s="48"/>
-      <c r="E14" s="49"/>
-      <c r="F14" s="36"/>
+      <c r="E14" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>36</v>
+      </c>
       <c r="G14" s="55"/>
       <c r="M14" t="s">
         <v>21</v>
@@ -2326,15 +2358,23 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="str">
+      <c r="A15" s="16">
         <f>IF(ISBLANK(B15),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B15))</f>
-        <v/>
-      </c>
-      <c r="B15" s="50"/>
+        <v>18</v>
+      </c>
+      <c r="B15" s="50">
+        <v>45775</v>
+      </c>
       <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="52">
+        <v>45</v>
+      </c>
+      <c r="E15" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="F15" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="G15" s="56"/>
       <c r="M15" t="s">
         <v>22</v>
@@ -8664,11 +8704,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8676,7 +8716,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>6.25E-2</v>
+        <v>0.13541666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8704,7 +8744,7 @@
       </c>
       <c r="B7">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C7,'Journal de travail'!$D$7:$D$532)</f>
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="C7" s="27" t="str">
         <f>'Journal de travail'!M11</f>
@@ -8712,7 +8752,7 @@
       </c>
       <c r="D7" s="33">
         <f t="shared" si="0"/>
-        <v>9.375E-2</v>
+        <v>0.11458333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -8793,7 +8833,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.38541666666666663</v>
+        <v>0.47916666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Ajout du dossier api
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_GolazNicola.xlsx
+++ b/Journal-de-Travail_GolazNicola.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po42oio\Documents\GitHub\P_appMaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA2DD64-ECEA-4311-AD2A-679D58986442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F20C6B3-8E20-47C3-A3A0-4EE8C077B518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="1335" yWindow="915" windowWidth="24630" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Début de l'affichage des livres, et recherche sur comment implémenter le backend</t>
+  </si>
+  <si>
+    <t>Création du conteneur docker pour la base de données, et fix de problème dans visual studio</t>
   </si>
 </sst>
 </file>
@@ -1085,7 +1088,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13541666666666666</c:v>
+                  <c:v>0.22916666666666666</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2020,7 +2023,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2073,7 +2076,7 @@
       </c>
       <c r="C3" s="22" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 9 heurs 0 minutes</v>
+        <v>0 jours 11 heurs 15 minutes</v>
       </c>
       <c r="D3" s="22"/>
       <c r="E3" s="3"/>
@@ -2088,15 +2091,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="22">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="D4" s="22">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="E4" s="40">
         <f>SUM(C4:D4)</f>
-        <v>540</v>
+        <v>675</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2387,15 +2390,25 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="str">
+      <c r="A16" s="8">
         <f>IF(ISBLANK(B16),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B16))</f>
-        <v/>
-      </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="B16" s="46">
+        <v>45782</v>
+      </c>
+      <c r="C16" s="47">
+        <v>2</v>
+      </c>
+      <c r="D16" s="48">
+        <v>15</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>38</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="O16">
         <v>40</v>
@@ -8704,11 +8717,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C5" s="41" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8716,7 +8729,7 @@
       </c>
       <c r="D5" s="33">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0.13541666666666666</v>
+        <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8833,7 +8846,7 @@
       </c>
       <c r="D12" s="34">
         <f>SUM(D4:D11)</f>
-        <v>0.47916666666666663</v>
+        <v>0.57291666666666663</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -9070,15 +9083,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9087,6 +9091,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9109,14 +9122,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9125,4 +9130,12 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Affichage de la liste de livre (fonctionne seulement sur emulateur)
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_GolazNicola.xlsx
+++ b/Journal-de-Travail_GolazNicola.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po42oio\Documents\GitHub\P_appMaui\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F20C6B3-8E20-47C3-A3A0-4EE8C077B518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF2A32A-E5B2-4D84-B076-717C6957E704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="915" windowWidth="24630" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="1680" yWindow="1260" windowWidth="24630" windowHeight="11385" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -2022,8 +2022,8 @@
   <dimension ref="A1:O532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2415,15 +2415,19 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="16" t="str">
+      <c r="A17" s="16">
         <f>IF(ISBLANK(B17),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B17))</f>
-        <v/>
-      </c>
-      <c r="B17" s="50"/>
+        <v>20</v>
+      </c>
+      <c r="B17" s="50">
+        <v>45789</v>
+      </c>
       <c r="C17" s="51"/>
       <c r="D17" s="52"/>
       <c r="E17" s="53"/>
-      <c r="F17" s="36"/>
+      <c r="F17" s="36" t="s">
+        <v>34</v>
+      </c>
       <c r="G17" s="56"/>
       <c r="O17">
         <v>45</v>
@@ -9083,6 +9087,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="be0d3259-a7ce-4623-88ec-81594dfcbc1c" xsi:nil="true"/>
@@ -9091,15 +9104,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9122,6 +9126,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -9130,12 +9142,4 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>